<commit_message>
Validacao Usuario, competencia, situacao
</commit_message>
<xml_diff>
--- a/Documentos/Cronograma.xlsx
+++ b/Documentos/Cronograma.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="160" windowWidth="23760" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Melhorias" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Caixa</t>
   </si>
@@ -94,16 +99,13 @@
   </si>
   <si>
     <t>Validar no banco cada campo</t>
-  </si>
-  <si>
-    <t>Modificar a estrutura de validação para MD5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +124,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,143 +175,145 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -330,9 +350,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -633,18 +655,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:H17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="8" width="12.7109375" customWidth="1"/>
+    <col min="2" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" thickBot="1"/>
+    <row r="4" spans="1:8">
       <c r="A4" s="14"/>
       <c r="B4" s="11" t="s">
         <v>15</v>
@@ -666,7 +688,7 @@
       </c>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -680,7 +702,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -694,7 +716,7 @@
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -714,13 +736,13 @@
         <v>0.9</v>
       </c>
       <c r="G7" s="7">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="H7" s="8">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -746,7 +768,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -760,7 +782,7 @@
       <c r="G9" s="5"/>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
         <v>3</v>
       </c>
@@ -786,11 +808,13 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
@@ -798,7 +822,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -812,7 +836,7 @@
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -826,7 +850,7 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
@@ -840,7 +864,7 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -854,7 +878,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -868,7 +892,7 @@
       <c r="G16" s="5"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -894,7 +918,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
         <v>11</v>
       </c>
@@ -906,7 +930,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -926,13 +950,13 @@
         <v>0.9</v>
       </c>
       <c r="G19" s="7">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H19" s="8">
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
         <v>13</v>
       </c>
@@ -944,7 +968,7 @@
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15" thickBot="1">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
@@ -964,7 +988,7 @@
         <v>0.9</v>
       </c>
       <c r="G21" s="9">
-        <v>0.9</v>
+        <v>0.95</v>
       </c>
       <c r="H21" s="10">
         <v>0.9</v>
@@ -981,7 +1005,12 @@
     <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -989,16 +1018,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
@@ -1006,17 +1035,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="16"/>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A3:A4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1026,8 +1057,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>